<commit_message>
added lstm neurons to attack features
</commit_message>
<xml_diff>
--- a/CIFAR-pytorch/CifarAttackmodels.xlsx
+++ b/CIFAR-pytorch/CifarAttackmodels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omars\OneDrive\Desktop\Research\Federated Learning\Implementations\time series\LSTM-MI\LSTM-MI\CIFAR-pytorch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F716EFE1-7BD8-4EFC-B810-F35F345832F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BCD16E-2009-4F42-9EA7-768E2E0D4A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{738F4FB1-DC9A-4149-A7D1-090D4C02DFBA}"/>
   </bookViews>
@@ -507,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA41839-586D-4771-9907-16622E0E2EB1}">
   <dimension ref="A1:AE49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U22" workbookViewId="0">
-      <selection activeCell="Z46" sqref="Z46:AE47"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -708,22 +708,22 @@
       <c r="Y2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA2">
+      <c r="Z2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA2" s="1">
         <v>0.63758683204650801</v>
       </c>
-      <c r="AB2">
+      <c r="AB2" s="1">
         <v>0.58244968188547797</v>
       </c>
-      <c r="AC2">
+      <c r="AC2" s="1">
         <v>0.97195512820512797</v>
       </c>
-      <c r="AD2">
+      <c r="AD2" s="1">
         <v>0.30321848290598202</v>
       </c>
-      <c r="AE2">
+      <c r="AE2" s="1">
         <v>0.72840093076788304</v>
       </c>
     </row>
@@ -803,22 +803,22 @@
       <c r="Y3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z3" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA3">
+      <c r="Z3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA3" s="1">
         <v>0.63721954822540205</v>
       </c>
-      <c r="AB3">
+      <c r="AB3" s="1">
         <v>0.58262967430639301</v>
       </c>
-      <c r="AC3">
+      <c r="AC3" s="1">
         <v>0.96754807692307598</v>
       </c>
-      <c r="AD3">
+      <c r="AD3" s="1">
         <v>0.30689102564102499</v>
       </c>
-      <c r="AE3">
+      <c r="AE3" s="1">
         <v>0.72730010540581203</v>
       </c>
     </row>
@@ -1016,22 +1016,22 @@
       <c r="Y6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z6" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA6">
+      <c r="Z6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA6" s="1">
         <v>0.62463271617889404</v>
       </c>
-      <c r="AB6">
+      <c r="AB6" s="1">
         <v>0.57573544329478599</v>
       </c>
-      <c r="AC6">
+      <c r="AC6" s="1">
         <v>0.94744925213675202</v>
       </c>
-      <c r="AD6">
+      <c r="AD6" s="1">
         <v>0.30181623931623902</v>
       </c>
-      <c r="AE6">
+      <c r="AE6" s="1">
         <v>0.71623633931500896</v>
       </c>
     </row>
@@ -1111,22 +1111,22 @@
       <c r="Y7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z7" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA7">
+      <c r="Z7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA7" s="1">
         <v>0.61995857954025202</v>
       </c>
-      <c r="AB7">
+      <c r="AB7" s="1">
         <v>0.57278878489526297</v>
       </c>
-      <c r="AC7">
+      <c r="AC7" s="1">
         <v>0.94397702991452903</v>
       </c>
-      <c r="AD7">
+      <c r="AD7" s="1">
         <v>0.29594017094017</v>
       </c>
-      <c r="AE7">
+      <c r="AE7" s="1">
         <v>0.71296366341377304</v>
       </c>
     </row>
@@ -1324,22 +1324,22 @@
       <c r="Y10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z10" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA10">
+      <c r="Z10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA10" s="1">
         <v>0.672876596450805</v>
       </c>
-      <c r="AB10">
+      <c r="AB10" s="1">
         <v>0.60452159870811395</v>
       </c>
-      <c r="AC10">
+      <c r="AC10" s="1">
         <v>0.99986645299145205</v>
       </c>
-      <c r="AD10">
+      <c r="AD10" s="1">
         <v>0.34588675213675202</v>
       </c>
-      <c r="AE10">
+      <c r="AE10" s="1">
         <v>0.753484627383887</v>
       </c>
     </row>
@@ -1419,22 +1419,22 @@
       <c r="Y11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z11" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA11">
+      <c r="Z11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA11" s="1">
         <v>0.67117387056350697</v>
       </c>
-      <c r="AB11">
+      <c r="AB11" s="1">
         <v>0.60337110367353497</v>
       </c>
-      <c r="AC11">
+      <c r="AC11" s="1">
         <v>0.99913194444444398</v>
       </c>
-      <c r="AD11">
+      <c r="AD11" s="1">
         <v>0.34321581196581102</v>
       </c>
-      <c r="AE11">
+      <c r="AE11" s="1">
         <v>0.752382149591451</v>
       </c>
     </row>
@@ -1632,22 +1632,22 @@
       <c r="Y14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z14" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA14">
+      <c r="Z14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA14" s="1">
         <v>0.66596555709838801</v>
       </c>
-      <c r="AB14">
+      <c r="AB14" s="1">
         <v>0.59954343385798303</v>
       </c>
-      <c r="AC14">
+      <c r="AC14" s="1">
         <v>0.99959935897435803</v>
       </c>
-      <c r="AD14">
+      <c r="AD14" s="1">
         <v>0.33233173076923</v>
       </c>
-      <c r="AE14">
+      <c r="AE14" s="1">
         <v>0.74953060458129905</v>
       </c>
     </row>
@@ -1727,22 +1727,22 @@
       <c r="Y15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z15" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA15">
+      <c r="Z15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA15" s="1">
         <v>0.65157586336135798</v>
       </c>
-      <c r="AB15">
+      <c r="AB15" s="1">
         <v>0.58936304228013503</v>
       </c>
-      <c r="AC15">
+      <c r="AC15" s="1">
         <v>0.99966613247863201</v>
       </c>
-      <c r="AD15">
+      <c r="AD15" s="1">
         <v>0.30348557692307598</v>
       </c>
-      <c r="AE15">
+      <c r="AE15" s="1">
         <v>0.74154242409232696</v>
       </c>
     </row>
@@ -1940,22 +1940,22 @@
       <c r="Y18" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z18" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA18">
+      <c r="Z18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA18" s="1">
         <v>0.66132479906082098</v>
       </c>
-      <c r="AB18">
+      <c r="AB18" s="1">
         <v>0.59625498007968103</v>
       </c>
-      <c r="AC18">
+      <c r="AC18" s="1">
         <v>0.99933226495726402</v>
       </c>
-      <c r="AD18">
+      <c r="AD18" s="1">
         <v>0.32331730769230699</v>
       </c>
-      <c r="AE18">
+      <c r="AE18" s="1">
         <v>0.74688092624014302</v>
       </c>
     </row>
@@ -2035,22 +2035,22 @@
       <c r="Y19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z19" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA19">
+      <c r="Z19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA19" s="1">
         <v>0.64807021617889404</v>
       </c>
-      <c r="AB19">
+      <c r="AB19" s="1">
         <v>0.58698466245636005</v>
       </c>
-      <c r="AC19">
+      <c r="AC19" s="1">
         <v>0.99919871794871795</v>
       </c>
-      <c r="AD19">
+      <c r="AD19" s="1">
         <v>0.29694177350427298</v>
       </c>
-      <c r="AE19">
+      <c r="AE19" s="1">
         <v>0.73952902221453398</v>
       </c>
     </row>
@@ -2248,22 +2248,22 @@
       <c r="Y22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z22" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA22">
+      <c r="Z22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA22" s="1">
         <v>0.68663191795349099</v>
       </c>
-      <c r="AB22">
+      <c r="AB22" s="1">
         <v>0.61477496714848801</v>
       </c>
-      <c r="AC22">
+      <c r="AC22" s="1">
         <v>0.99966613247863201</v>
       </c>
-      <c r="AD22">
+      <c r="AD22" s="1">
         <v>0.373597756410256</v>
       </c>
-      <c r="AE22">
+      <c r="AE22" s="1">
         <v>0.76134052074857606</v>
       </c>
     </row>
@@ -2343,22 +2343,22 @@
       <c r="Y23" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z23" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA23">
+      <c r="Z23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA23" s="1">
         <v>0.68930286169052102</v>
       </c>
-      <c r="AB23">
+      <c r="AB23" s="1">
         <v>0.61681087762669895</v>
       </c>
-      <c r="AC23">
+      <c r="AC23" s="1">
         <v>0.99959935897435803</v>
       </c>
-      <c r="AD23">
+      <c r="AD23" s="1">
         <v>0.37900641025641002</v>
       </c>
-      <c r="AE23">
+      <c r="AE23" s="1">
         <v>0.76288029353309805</v>
       </c>
     </row>
@@ -2556,22 +2556,22 @@
       <c r="Y26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z26" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA26">
+      <c r="Z26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA26" s="1">
         <v>0.60209667682647705</v>
       </c>
-      <c r="AB26">
+      <c r="AB26" s="1">
         <v>0.55973122900226502</v>
       </c>
-      <c r="AC26">
+      <c r="AC26" s="1">
         <v>0.95673076923076905</v>
       </c>
-      <c r="AD26">
+      <c r="AD26" s="1">
         <v>0.24746260683760599</v>
       </c>
-      <c r="AE26">
+      <c r="AE26" s="1">
         <v>0.70626509587420505</v>
       </c>
     </row>
@@ -2651,22 +2651,22 @@
       <c r="Y27" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z27" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA27">
+      <c r="Z27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA27" s="1">
         <v>0.60286456346511796</v>
       </c>
-      <c r="AB27">
+      <c r="AB27" s="1">
         <v>0.5597764929572</v>
       </c>
-      <c r="AC27">
+      <c r="AC27" s="1">
         <v>0.96327457264957195</v>
       </c>
-      <c r="AD27">
+      <c r="AD27" s="1">
         <v>0.24245459401709399</v>
       </c>
-      <c r="AE27">
+      <c r="AE27" s="1">
         <v>0.70807666822097304</v>
       </c>
     </row>
@@ -2864,22 +2864,22 @@
       <c r="Y30" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z30" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA30">
+      <c r="Z30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA30" s="1">
         <v>0.60386615991592396</v>
       </c>
-      <c r="AB30">
+      <c r="AB30" s="1">
         <v>0.56093548007991501</v>
       </c>
-      <c r="AC30">
+      <c r="AC30" s="1">
         <v>0.95612980769230704</v>
       </c>
-      <c r="AD30">
+      <c r="AD30" s="1">
         <v>0.25160256410256399</v>
       </c>
-      <c r="AE30">
+      <c r="AE30" s="1">
         <v>0.70705873638989603</v>
       </c>
     </row>
@@ -2959,22 +2959,22 @@
       <c r="Y31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z31" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA31">
+      <c r="Z31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA31" s="1">
         <v>0.60820645093917802</v>
       </c>
-      <c r="AB31">
+      <c r="AB31" s="1">
         <v>0.56280277487113906</v>
       </c>
-      <c r="AC31">
+      <c r="AC31" s="1">
         <v>0.969684829059829</v>
       </c>
-      <c r="AD31">
+      <c r="AD31" s="1">
         <v>0.246728098290598</v>
       </c>
-      <c r="AE31">
+      <c r="AE31" s="1">
         <v>0.71222933372569197</v>
       </c>
     </row>
@@ -3172,22 +3172,22 @@
       <c r="Y34" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z34" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA34">
+      <c r="Z34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA34" s="1">
         <v>0.57922679185867298</v>
       </c>
-      <c r="AB34">
+      <c r="AB34" s="1">
         <v>0.55226181561908105</v>
       </c>
-      <c r="AC34">
+      <c r="AC34" s="1">
         <v>0.83720619658119599</v>
       </c>
-      <c r="AD34">
+      <c r="AD34" s="1">
         <v>0.321247329059829</v>
       </c>
-      <c r="AE34">
+      <c r="AE34" s="1">
         <v>0.66551660075904295</v>
       </c>
     </row>
@@ -3267,22 +3267,22 @@
       <c r="Y35" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z35" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA35">
+      <c r="Z35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA35" s="1">
         <v>0.58807426691055298</v>
       </c>
-      <c r="AB35">
+      <c r="AB35" s="1">
         <v>0.54984506084196205</v>
       </c>
-      <c r="AC35">
+      <c r="AC35" s="1">
         <v>0.971554487179487</v>
       </c>
-      <c r="AD35">
+      <c r="AD35" s="1">
         <v>0.20459401709401701</v>
       </c>
-      <c r="AE35">
+      <c r="AE35" s="1">
         <v>0.70225396978618604</v>
       </c>
     </row>
@@ -3480,22 +3480,22 @@
       <c r="Y38" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z38" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA38">
+      <c r="Z38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA38" s="1">
         <v>0.64950585365295399</v>
       </c>
-      <c r="AB38">
+      <c r="AB38" s="1">
         <v>0.58790043969849204</v>
       </c>
-      <c r="AC38">
+      <c r="AC38" s="1">
         <v>0.99993322649572602</v>
       </c>
-      <c r="AD38">
+      <c r="AD38" s="1">
         <v>0.29907852564102499</v>
       </c>
-      <c r="AE38">
+      <c r="AE38" s="1">
         <v>0.740456882911392</v>
       </c>
     </row>
@@ -3575,22 +3575,22 @@
       <c r="Y39" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z39" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA39">
+      <c r="Z39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA39" s="1">
         <v>0.63785392045974698</v>
       </c>
-      <c r="AB39">
+      <c r="AB39" s="1">
         <v>0.58044655730039296</v>
       </c>
-      <c r="AC39">
+      <c r="AC39" s="1">
         <v>0.99465811965811901</v>
       </c>
-      <c r="AD39">
+      <c r="AD39" s="1">
         <v>0.28104967948717902</v>
       </c>
-      <c r="AE39">
+      <c r="AE39" s="1">
         <v>0.73308890474667099</v>
       </c>
     </row>
@@ -3788,22 +3788,22 @@
       <c r="Y42" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z42" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA42">
+      <c r="Z42" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA42" s="1">
         <v>0.6640625</v>
       </c>
-      <c r="AB42">
+      <c r="AB42" s="1">
         <v>0.59813084112149495</v>
       </c>
-      <c r="AC42">
-        <v>1</v>
-      </c>
-      <c r="AD42">
+      <c r="AC42" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD42" s="1">
         <v>0.328125</v>
       </c>
-      <c r="AE42">
+      <c r="AE42" s="1">
         <v>0.74853801169590595</v>
       </c>
     </row>
@@ -3883,22 +3883,22 @@
       <c r="Y43" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z43" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA43">
+      <c r="Z43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA43" s="1">
         <v>0.62513357400894098</v>
       </c>
-      <c r="AB43">
+      <c r="AB43" s="1">
         <v>0.57427076727964399</v>
       </c>
-      <c r="AC43">
+      <c r="AC43" s="1">
         <v>0.96754807692307598</v>
       </c>
-      <c r="AD43">
+      <c r="AD43" s="1">
         <v>0.28271901709401698</v>
       </c>
-      <c r="AE43">
+      <c r="AE43" s="1">
         <v>0.72075208913649003</v>
       </c>
     </row>
@@ -4096,22 +4096,22 @@
       <c r="Y46" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z46" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA46">
+      <c r="Z46" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA46" s="1">
         <v>0.61675345897674505</v>
       </c>
-      <c r="AB46">
+      <c r="AB46" s="1">
         <v>0.56841569824314198</v>
       </c>
-      <c r="AC46">
+      <c r="AC46" s="1">
         <v>0.97001869658119599</v>
       </c>
-      <c r="AD46">
+      <c r="AD46" s="1">
         <v>0.26348824786324698</v>
       </c>
-      <c r="AE46">
+      <c r="AE46" s="1">
         <v>0.71679865788369901</v>
       </c>
     </row>
@@ -4191,22 +4191,22 @@
       <c r="Y47" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="Z47" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA47">
+      <c r="Z47" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA47" s="1">
         <v>0.61651974916458097</v>
       </c>
-      <c r="AB47">
+      <c r="AB47" s="1">
         <v>0.56840991061627699</v>
       </c>
-      <c r="AC47">
+      <c r="AC47" s="1">
         <v>0.96814903846153799</v>
       </c>
-      <c r="AD47">
+      <c r="AD47" s="1">
         <v>0.26489049145299098</v>
       </c>
-      <c r="AE47">
+      <c r="AE47" s="1">
         <v>0.71628297599051405</v>
       </c>
     </row>

</xml_diff>

<commit_message>
edit rnn stl10 pipeline
</commit_message>
<xml_diff>
--- a/CIFAR-pytorch/CifarAttackmodels.xlsx
+++ b/CIFAR-pytorch/CifarAttackmodels.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omars\OneDrive\Desktop\Research\Federated Learning\Implementations\time series\LSTM-MI\LSTM-MI\CIFAR-pytorch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BCD16E-2009-4F42-9EA7-768E2E0D4A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1518BF8F-C5A5-4EC0-A368-10B80237A0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{738F4FB1-DC9A-4149-A7D1-090D4C02DFBA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="30">
   <si>
     <t>Model</t>
   </si>
@@ -111,12 +111,6 @@
   </si>
   <si>
     <t>ResNet20</t>
-  </si>
-  <si>
-    <t>DenseNet122</t>
-  </si>
-  <si>
-    <t>DenseNet123</t>
   </si>
   <si>
     <t>Attack model</t>
@@ -507,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA41839-586D-4771-9907-16622E0E2EB1}">
   <dimension ref="A1:AE49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -563,7 +557,7 @@
         <v>0</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>1</v>
@@ -587,7 +581,7 @@
         <v>0</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>1</v>
@@ -611,7 +605,7 @@
         <v>0</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>1</v>
@@ -632,7 +626,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -655,10 +649,10 @@
         <v>0.99719316022635096</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>20</v>
@@ -679,10 +673,10 @@
         <v>0.75459898900411604</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>20</v>
@@ -703,10 +697,10 @@
         <v>0.74907148308318505</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z2" s="1" t="s">
         <v>20</v>
@@ -727,7 +721,7 @@
         <v>0.72840093076788304</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -750,10 +744,10 @@
         <v>0.74556804221508599</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>19</v>
@@ -774,10 +768,10 @@
         <v>0.75410864055600502</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>19</v>
@@ -798,10 +792,10 @@
         <v>0.74853562878826396</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z3" s="1" t="s">
         <v>19</v>
@@ -822,7 +816,7 @@
         <v>0.72730010540581203</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -845,10 +839,10 @@
         <v>0.997404183600201</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -857,10 +851,10 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
@@ -869,10 +863,10 @@
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
@@ -881,7 +875,7 @@
       <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -904,10 +898,10 @@
         <v>0.74313334827328004</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -916,10 +910,10 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
@@ -928,10 +922,10 @@
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
       <c r="X5" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
@@ -940,7 +934,7 @@
       <c r="AD5" s="1"/>
       <c r="AE5" s="1"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -963,10 +957,10 @@
         <v>0.99052778873828795</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>20</v>
@@ -987,10 +981,10 @@
         <v>0.743608435303306</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>20</v>
@@ -1011,10 +1005,10 @@
         <v>0.74144437883494596</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z6" s="1" t="s">
         <v>20</v>
@@ -1035,7 +1029,7 @@
         <v>0.71623633931500896</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1058,10 +1052,10 @@
         <v>0.73469723392862596</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>19</v>
@@ -1082,10 +1076,10 @@
         <v>0.74158766538180998</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>19</v>
@@ -1106,10 +1100,10 @@
         <v>0.740179328417645</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z7" s="1" t="s">
         <v>19</v>
@@ -1130,7 +1124,7 @@
         <v>0.71296366341377304</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1153,10 +1147,10 @@
         <v>0.98813181537486505</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -1165,10 +1159,10 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
@@ -1177,10 +1171,10 @@
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1"/>
@@ -1189,7 +1183,7 @@
       <c r="AD8" s="1"/>
       <c r="AE8" s="1"/>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1212,10 +1206,10 @@
         <v>0.739417423790106</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1224,10 +1218,10 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
@@ -1236,10 +1230,10 @@
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y9" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
@@ -1248,7 +1242,7 @@
       <c r="AD9" s="1"/>
       <c r="AE9" s="1"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1271,10 +1265,10 @@
         <v>1</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>20</v>
@@ -1295,10 +1289,10 @@
         <v>0.77510029765756405</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>20</v>
@@ -1319,10 +1313,10 @@
         <v>0.76105295253582605</v>
       </c>
       <c r="X10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z10" s="1" t="s">
         <v>20</v>
@@ -1343,7 +1337,7 @@
         <v>0.753484627383887</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1366,10 +1360,10 @@
         <v>0.75505274336900796</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>19</v>
@@ -1390,10 +1384,10 @@
         <v>0.77332988758237498</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R11" s="1" t="s">
         <v>19</v>
@@ -1414,10 +1408,10 @@
         <v>0.75927991886409696</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z11" s="1" t="s">
         <v>19</v>
@@ -1438,7 +1432,7 @@
         <v>0.752382149591451</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -1461,10 +1455,10 @@
         <v>1</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -1473,10 +1467,10 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
@@ -1485,10 +1479,10 @@
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z12" s="1"/>
       <c r="AA12" s="1"/>
@@ -1497,7 +1491,7 @@
       <c r="AD12" s="1"/>
       <c r="AE12" s="1"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1520,10 +1514,10 @@
         <v>0.74414315932646602</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1532,10 +1526,10 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
@@ -1544,10 +1538,10 @@
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
@@ -1556,7 +1550,7 @@
       <c r="AD13" s="1"/>
       <c r="AE13" s="1"/>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1579,10 +1573,10 @@
         <v>1</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>20</v>
@@ -1603,10 +1597,10 @@
         <v>0.77521307738141498</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R14" s="1" t="s">
         <v>20</v>
@@ -1627,10 +1621,10 @@
         <v>0.76450616496055901</v>
       </c>
       <c r="X14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z14" s="1" t="s">
         <v>20</v>
@@ -1651,7 +1645,7 @@
         <v>0.74953060458129905</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -1674,10 +1668,10 @@
         <v>0.77117797570225</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>19</v>
@@ -1698,10 +1692,10 @@
         <v>0.767341077518783</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R15" s="1" t="s">
         <v>19</v>
@@ -1722,10 +1716,10 @@
         <v>0.75897903834942804</v>
       </c>
       <c r="X15" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z15" s="1" t="s">
         <v>19</v>
@@ -1746,7 +1740,7 @@
         <v>0.74154242409232696</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
@@ -1769,10 +1763,10 @@
         <v>1</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -1781,10 +1775,10 @@
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
@@ -1793,10 +1787,10 @@
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
@@ -1805,7 +1799,7 @@
       <c r="AD16" s="1"/>
       <c r="AE16" s="1"/>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>10</v>
       </c>
@@ -1828,10 +1822,10 @@
         <v>0.76031896184218395</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -1840,10 +1834,10 @@
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
@@ -1852,10 +1846,10 @@
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
       <c r="X17" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y17" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
@@ -1864,7 +1858,7 @@
       <c r="AD17" s="1"/>
       <c r="AE17" s="1"/>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
@@ -1887,10 +1881,10 @@
         <v>1</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>20</v>
@@ -1911,10 +1905,10 @@
         <v>0.76751461688378297</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R18" s="1" t="s">
         <v>20</v>
@@ -1935,10 +1929,10 @@
         <v>0.75768539837562898</v>
       </c>
       <c r="X18" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z18" s="1" t="s">
         <v>20</v>
@@ -1959,7 +1953,7 @@
         <v>0.74688092624014302</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
@@ -1982,10 +1976,10 @@
         <v>0.76095272086117405</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>19</v>
@@ -2006,10 +2000,10 @@
         <v>0.76280515773915702</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R19" s="1" t="s">
         <v>19</v>
@@ -2030,10 +2024,10 @@
         <v>0.75443369609028599</v>
       </c>
       <c r="X19" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y19" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z19" s="1" t="s">
         <v>19</v>
@@ -2054,7 +2048,7 @@
         <v>0.73952902221453398</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>11</v>
       </c>
@@ -2077,10 +2071,10 @@
         <v>1</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -2089,10 +2083,10 @@
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
@@ -2101,10 +2095,10 @@
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
       <c r="X20" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y20" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z20" s="1"/>
       <c r="AA20" s="1"/>
@@ -2113,7 +2107,7 @@
       <c r="AD20" s="1"/>
       <c r="AE20" s="1"/>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
@@ -2136,10 +2130,10 @@
         <v>0.76114956793124</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -2148,10 +2142,10 @@
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
@@ -2160,10 +2154,10 @@
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
       <c r="X21" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y21" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z21" s="1"/>
       <c r="AA21" s="1"/>
@@ -2172,7 +2166,7 @@
       <c r="AD21" s="1"/>
       <c r="AE21" s="1"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>12</v>
       </c>
@@ -2195,10 +2189,10 @@
         <v>1</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>20</v>
@@ -2219,10 +2213,10 @@
         <v>0.77388181183948701</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R22" s="1" t="s">
         <v>20</v>
@@ -2243,10 +2237,10 @@
         <v>0.76342688180265605</v>
       </c>
       <c r="X22" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y22" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z22" s="1" t="s">
         <v>20</v>
@@ -2267,7 +2261,7 @@
         <v>0.76134052074857606</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
@@ -2290,10 +2284,10 @@
         <v>0.75323951036162295</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>19</v>
@@ -2314,10 +2308,10 @@
         <v>0.77380183438832195</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R23" s="1" t="s">
         <v>19</v>
@@ -2338,10 +2332,10 @@
         <v>0.76373093987454699</v>
       </c>
       <c r="X23" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y23" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z23" s="1" t="s">
         <v>19</v>
@@ -2362,7 +2356,7 @@
         <v>0.76288029353309805</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -2385,10 +2379,10 @@
         <v>1</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -2397,10 +2391,10 @@
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
@@ -2409,10 +2403,10 @@
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
       <c r="X24" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y24" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
@@ -2421,7 +2415,7 @@
       <c r="AD24" s="1"/>
       <c r="AE24" s="1"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -2444,10 +2438,10 @@
         <v>0.75564815565379495</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -2456,10 +2450,10 @@
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
@@ -2468,10 +2462,10 @@
       <c r="V25" s="1"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y25" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
@@ -2503,34 +2497,34 @@
         <v>0.99510786206179003</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>20</v>
       </c>
       <c r="K26" s="1">
-        <v>0.63434827327728205</v>
+        <v>0.64383012056350697</v>
       </c>
       <c r="L26" s="1">
-        <v>0.58204877253078802</v>
+        <v>0.58931088813334398</v>
       </c>
       <c r="M26" s="1">
-        <v>0.95305822649572602</v>
+        <v>0.949051816239316</v>
       </c>
       <c r="N26" s="1">
-        <v>0.315638354700854</v>
+        <v>0.33860844017093999</v>
       </c>
       <c r="O26" s="1">
-        <v>0.72272013772849197</v>
+        <v>0.72711925103596398</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R26" s="1" t="s">
         <v>20</v>
@@ -2551,10 +2545,10 @@
         <v>0.72160256089631303</v>
       </c>
       <c r="X26" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y26" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z26" s="1" t="s">
         <v>20</v>
@@ -2598,34 +2592,34 @@
         <v>0.80652956403989595</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K27" s="1">
-        <v>0.63955664634704501</v>
+        <v>0.64072513580322199</v>
       </c>
       <c r="L27" s="1">
-        <v>0.58495244289082104</v>
+        <v>0.587970113119338</v>
       </c>
       <c r="M27" s="1">
-        <v>0.9609375</v>
+        <v>0.94057158119658102</v>
       </c>
       <c r="N27" s="1">
-        <v>0.31817574786324698</v>
+        <v>0.34087873931623902</v>
       </c>
       <c r="O27" s="1">
-        <v>0.72722219414826395</v>
+        <v>0.72360208563429396</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R27" s="1" t="s">
         <v>19</v>
@@ -2646,10 +2640,10 @@
         <v>0.72614522904580903</v>
       </c>
       <c r="X27" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y27" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z27" s="1" t="s">
         <v>19</v>
@@ -2693,10 +2687,10 @@
         <v>0.99463608434105499</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -2705,10 +2699,10 @@
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
@@ -2717,10 +2711,10 @@
       <c r="V28" s="1"/>
       <c r="W28" s="1"/>
       <c r="X28" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y28" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z28" s="1"/>
       <c r="AA28" s="1"/>
@@ -2752,10 +2746,10 @@
         <v>0.81241162093443897</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -2764,10 +2758,10 @@
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
@@ -2776,10 +2770,10 @@
       <c r="V29" s="1"/>
       <c r="W29" s="1"/>
       <c r="X29" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y29" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z29" s="1"/>
       <c r="AA29" s="1"/>
@@ -2811,34 +2805,34 @@
         <v>0.99695770709304399</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>20</v>
       </c>
       <c r="K30" s="1">
-        <v>0.63267892599105802</v>
+        <v>0.65064102411270097</v>
       </c>
       <c r="L30" s="1">
-        <v>0.57924543351679003</v>
+        <v>0.59598366235534295</v>
       </c>
       <c r="M30" s="1">
-        <v>0.96981837606837595</v>
+        <v>0.93536324786324698</v>
       </c>
       <c r="N30" s="1">
-        <v>0.29553952991452898</v>
+        <v>0.36591880341880301</v>
       </c>
       <c r="O30" s="1">
-        <v>0.72529338327091097</v>
+        <v>0.72806652806652805</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R30" s="1" t="s">
         <v>20</v>
@@ -2859,10 +2853,10 @@
         <v>0.72418937736224398</v>
       </c>
       <c r="X30" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y30" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z30" s="1" t="s">
         <v>20</v>
@@ -2906,34 +2900,34 @@
         <v>0.80944941014190497</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K31" s="1">
-        <v>0.63568377494812001</v>
+        <v>0.64232772588729803</v>
       </c>
       <c r="L31" s="1">
-        <v>0.58051989221746703</v>
+        <v>0.595024742543801</v>
       </c>
       <c r="M31" s="1">
-        <v>0.97823183760683696</v>
+        <v>0.89122596153846101</v>
       </c>
       <c r="N31" s="1">
-        <v>0.293135683760683</v>
+        <v>0.393429487179487</v>
       </c>
       <c r="O31" s="1">
-        <v>0.72863821744752799</v>
+        <v>0.713609752185419</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R31" s="1" t="s">
         <v>19</v>
@@ -2954,10 +2948,10 @@
         <v>0.72770499517075704</v>
       </c>
       <c r="X31" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y31" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z31" s="1" t="s">
         <v>19</v>
@@ -3001,10 +2995,10 @@
         <v>0.99452335916941803</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -3013,10 +3007,10 @@
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
       <c r="P32" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
@@ -3025,10 +3019,10 @@
       <c r="V32" s="1"/>
       <c r="W32" s="1"/>
       <c r="X32" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y32" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z32" s="1"/>
       <c r="AA32" s="1"/>
@@ -3060,10 +3054,10 @@
         <v>0.81093135131951399</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -3072,10 +3066,10 @@
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
       <c r="P33" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
@@ -3084,10 +3078,10 @@
       <c r="V33" s="1"/>
       <c r="W33" s="1"/>
       <c r="X33" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y33" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z33" s="1"/>
       <c r="AA33" s="1"/>
@@ -3119,34 +3113,34 @@
         <v>0.99501003383974795</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>20</v>
       </c>
       <c r="K34" s="1">
-        <v>0.61167865991592396</v>
+        <v>0.60803955793380704</v>
       </c>
       <c r="L34" s="1">
-        <v>0.57146519676964402</v>
+        <v>0.57156758669497498</v>
       </c>
       <c r="M34" s="1">
-        <v>0.89302884615384603</v>
+        <v>0.86284722222222199</v>
       </c>
       <c r="N34" s="1">
-        <v>0.33032852564102499</v>
+        <v>0.35323183760683702</v>
       </c>
       <c r="O34" s="1">
-        <v>0.69694364105370099</v>
+        <v>0.68763303533418396</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R34" s="1" t="s">
         <v>20</v>
@@ -3167,10 +3161,10 @@
         <v>0.69373774349588102</v>
       </c>
       <c r="X34" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y34" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z34" s="1" t="s">
         <v>20</v>
@@ -3214,34 +3208,34 @@
         <v>0.79714706667290403</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K35" s="1">
-        <v>0.62336403131484897</v>
+        <v>0.62937366962432795</v>
       </c>
       <c r="L35" s="1">
-        <v>0.57194034500214097</v>
+        <v>0.57617456261057598</v>
       </c>
       <c r="M35" s="1">
-        <v>0.98076923076922995</v>
+        <v>0.97856570512820495</v>
       </c>
       <c r="N35" s="1">
-        <v>0.26595886752136699</v>
+        <v>0.28018162393162299</v>
       </c>
       <c r="O35" s="1">
-        <v>0.72253240524386897</v>
+        <v>0.72529756749399898</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R35" s="1" t="s">
         <v>19</v>
@@ -3262,10 +3256,10 @@
         <v>0.72288978990047903</v>
       </c>
       <c r="X35" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y35" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z35" s="1" t="s">
         <v>19</v>
@@ -3288,7 +3282,7 @@
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>22</v>
@@ -3309,10 +3303,10 @@
         <v>0.95602527030245898</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
@@ -3321,10 +3315,10 @@
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
@@ -3333,10 +3327,10 @@
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
       <c r="X36" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y36" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z36" s="1"/>
       <c r="AA36" s="1"/>
@@ -3347,7 +3341,7 @@
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>22</v>
@@ -3368,10 +3362,10 @@
         <v>0.77763415340494901</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
@@ -3380,10 +3374,10 @@
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
       <c r="P37" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R37" s="1"/>
       <c r="S37" s="1"/>
@@ -3392,10 +3386,10 @@
       <c r="V37" s="1"/>
       <c r="W37" s="1"/>
       <c r="X37" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y37" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z37" s="1"/>
       <c r="AA37" s="1"/>
@@ -3427,34 +3421,34 @@
         <v>0.99966900565828498</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>20</v>
       </c>
       <c r="K38" s="1">
-        <v>0.68396103382110596</v>
+        <v>0.728565692901611</v>
       </c>
       <c r="L38" s="1">
-        <v>0.612715817036249</v>
+        <v>0.65077966698969203</v>
       </c>
       <c r="M38" s="1">
-        <v>1</v>
+        <v>0.98651175213675202</v>
       </c>
       <c r="N38" s="1">
-        <v>0.36792200854700802</v>
+        <v>0.470619658119658</v>
       </c>
       <c r="O38" s="1">
-        <v>0.75985590339438802</v>
+        <v>0.78422421572270296</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R38" s="1" t="s">
         <v>20</v>
@@ -3475,10 +3469,10 @@
         <v>0.75043219001327799</v>
       </c>
       <c r="X38" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y38" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z38" s="1" t="s">
         <v>20</v>
@@ -3522,34 +3516,34 @@
         <v>0.75999150533981197</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K39" s="1">
-        <v>0.68092280626296997</v>
+        <v>0.73150372505187899</v>
       </c>
       <c r="L39" s="1">
-        <v>0.61103143056181597</v>
+        <v>0.65312251567882695</v>
       </c>
       <c r="M39" s="1">
-        <v>0.99565972222222199</v>
+        <v>0.98744658119658102</v>
       </c>
       <c r="N39" s="1">
-        <v>0.36618589743589702</v>
+        <v>0.47556089743589702</v>
       </c>
       <c r="O39" s="1">
-        <v>0.75730719418979597</v>
+        <v>0.78621936307087004</v>
       </c>
       <c r="P39" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R39" s="1" t="s">
         <v>19</v>
@@ -3570,10 +3564,10 @@
         <v>0.75017564990464702</v>
       </c>
       <c r="X39" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y39" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z39" s="1" t="s">
         <v>19</v>
@@ -3617,10 +3611,10 @@
         <v>1</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
@@ -3629,10 +3623,10 @@
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
       <c r="P40" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R40" s="1"/>
       <c r="S40" s="1"/>
@@ -3641,10 +3635,10 @@
       <c r="V40" s="1"/>
       <c r="W40" s="1"/>
       <c r="X40" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y40" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z40" s="1"/>
       <c r="AA40" s="1"/>
@@ -3676,10 +3670,10 @@
         <v>0.76997223838624695</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
@@ -3688,10 +3682,10 @@
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
       <c r="P41" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R41" s="1"/>
       <c r="S41" s="1"/>
@@ -3700,10 +3694,10 @@
       <c r="V41" s="1"/>
       <c r="W41" s="1"/>
       <c r="X41" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y41" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z41" s="1"/>
       <c r="AA41" s="1"/>
@@ -3735,34 +3729,34 @@
         <v>0.99680627191537596</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>20</v>
       </c>
       <c r="K42" s="1">
-        <v>0.69093883037567105</v>
+        <v>0.70382612943649203</v>
       </c>
       <c r="L42" s="1">
-        <v>0.61800024759625305</v>
+        <v>0.63283867879368105</v>
       </c>
       <c r="M42" s="1">
-        <v>1</v>
+        <v>0.97102029914529897</v>
       </c>
       <c r="N42" s="1">
-        <v>0.38187767094017</v>
+        <v>0.43663194444444398</v>
       </c>
       <c r="O42" s="1">
-        <v>0.76390624601494495</v>
+        <v>0.76627585298379597</v>
       </c>
       <c r="P42" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q42" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R42" s="1" t="s">
         <v>20</v>
@@ -3783,10 +3777,10 @@
         <v>0.75474360589643397</v>
       </c>
       <c r="X42" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y42" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z42" s="1" t="s">
         <v>20</v>
@@ -3830,34 +3824,34 @@
         <v>0.74828824248733194</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K43" s="1">
-        <v>0.670873403549194</v>
+        <v>0.71624600887298495</v>
       </c>
       <c r="L43" s="1">
-        <v>0.60674063568866199</v>
+        <v>0.64026159643120095</v>
       </c>
       <c r="M43" s="1">
-        <v>0.97128739316239299</v>
+        <v>0.98711271367521303</v>
       </c>
       <c r="N43" s="1">
-        <v>0.370459401709401</v>
+        <v>0.44537927350427298</v>
       </c>
       <c r="O43" s="1">
-        <v>0.746906290115532</v>
+        <v>0.776724024694601</v>
       </c>
       <c r="P43" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R43" s="1" t="s">
         <v>19</v>
@@ -3878,10 +3872,10 @@
         <v>0.74466519499632</v>
       </c>
       <c r="X43" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y43" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z43" s="1" t="s">
         <v>19</v>
@@ -3925,10 +3919,10 @@
         <v>1</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
@@ -3937,10 +3931,10 @@
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
       <c r="P44" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
@@ -3949,10 +3943,10 @@
       <c r="V44" s="1"/>
       <c r="W44" s="1"/>
       <c r="X44" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y44" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z44" s="1"/>
       <c r="AA44" s="1"/>
@@ -3984,10 +3978,10 @@
         <v>0.77506421535693304</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
@@ -3996,10 +3990,10 @@
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
       <c r="P45" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R45" s="1"/>
       <c r="S45" s="1"/>
@@ -4008,10 +4002,10 @@
       <c r="V45" s="1"/>
       <c r="W45" s="1"/>
       <c r="X45" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y45" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z45" s="1"/>
       <c r="AA45" s="1"/>
@@ -4043,34 +4037,34 @@
         <v>0.99706418609453096</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>20</v>
       </c>
       <c r="K46" s="1">
-        <v>0.66266024112701405</v>
+        <v>0.68676549196243197</v>
       </c>
       <c r="L46" s="1">
-        <v>0.60016447368421</v>
+        <v>0.64402677651905205</v>
       </c>
       <c r="M46" s="1">
-        <v>0.97462606837606802</v>
+        <v>0.83513621794871795</v>
       </c>
       <c r="N46" s="1">
-        <v>0.35069444444444398</v>
+        <v>0.53839476495726402</v>
       </c>
       <c r="O46" s="1">
-        <v>0.74287459283387602</v>
+        <v>0.727235725084312</v>
       </c>
       <c r="P46" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R46" s="1" t="s">
         <v>20</v>
@@ -4091,10 +4085,10 @@
         <v>0.73988526570048296</v>
       </c>
       <c r="X46" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y46" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z46" s="1" t="s">
         <v>20</v>
@@ -4138,34 +4132,34 @@
         <v>0.75141136857129798</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K47" s="1">
-        <v>0.66549813747405995</v>
+        <v>0.69140625</v>
       </c>
       <c r="L47" s="1">
-        <v>0.60201687590039099</v>
+        <v>0.64691712367382503</v>
       </c>
       <c r="M47" s="1">
-        <v>0.97662927350427298</v>
+        <v>0.84281517094017</v>
       </c>
       <c r="N47" s="1">
-        <v>0.354366987179487</v>
+        <v>0.539997329059829</v>
       </c>
       <c r="O47" s="1">
-        <v>0.74487535331415</v>
+        <v>0.73198596572621499</v>
       </c>
       <c r="P47" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q47" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R47" s="1" t="s">
         <v>19</v>
@@ -4186,10 +4180,10 @@
         <v>0.74155723504155402</v>
       </c>
       <c r="X47" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y47" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z47" s="1" t="s">
         <v>19</v>
@@ -4233,10 +4227,10 @@
         <v>0.99352827128403698</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
@@ -4245,10 +4239,10 @@
       <c r="N48" s="1"/>
       <c r="O48" s="1"/>
       <c r="P48" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q48" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R48" s="1"/>
       <c r="S48" s="1"/>
@@ -4257,10 +4251,10 @@
       <c r="V48" s="1"/>
       <c r="W48" s="1"/>
       <c r="X48" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y48" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z48" s="1"/>
       <c r="AA48" s="1"/>
@@ -4292,10 +4286,10 @@
         <v>0.74588403689574601</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
@@ -4304,10 +4298,10 @@
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
       <c r="P49" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Q49" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="R49" s="1"/>
       <c r="S49" s="1"/>
@@ -4316,10 +4310,10 @@
       <c r="V49" s="1"/>
       <c r="W49" s="1"/>
       <c r="X49" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="Y49" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="Z49" s="1"/>
       <c r="AA49" s="1"/>

</xml_diff>